<commit_message>
added cutest vampire ever
</commit_message>
<xml_diff>
--- a/evakuu.xlsx
+++ b/evakuu.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="375">
   <si>
     <t>overlord_(maruyama)</t>
   </si>
@@ -1135,6 +1135,12 @@
   </si>
   <si>
     <t>niji_(rudduf232)</t>
+  </si>
+  <si>
+    <t>remilia_scarlet</t>
+  </si>
+  <si>
+    <t>touhou</t>
   </si>
 </sst>
 </file>
@@ -1479,10 +1485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E361"/>
+  <dimension ref="A1:E362"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A170" sqref="A170"/>
+    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
+      <selection activeCell="D267" sqref="D267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4435,18 +4441,21 @@
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
-        <v>84</v>
+        <v>373</v>
       </c>
       <c r="B266" s="1" t="s">
         <v>270</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
+      </c>
+      <c r="D266" s="1" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>215</v>
+        <v>84</v>
       </c>
       <c r="B267" s="1" t="s">
         <v>270</v>
@@ -4457,7 +4466,7 @@
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>194</v>
+        <v>215</v>
       </c>
       <c r="B268" s="1" t="s">
         <v>270</v>
@@ -4468,35 +4477,35 @@
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>49</v>
+        <v>194</v>
       </c>
       <c r="B269" s="1" t="s">
         <v>270</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D269" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="E269" s="1" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
-        <v>243</v>
+        <v>49</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>270</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
+      </c>
+      <c r="D270" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E270" s="1" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
-        <v>93</v>
+        <v>243</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>270</v>
@@ -4507,7 +4516,7 @@
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
-        <v>142</v>
+        <v>93</v>
       </c>
       <c r="B272" s="1" t="s">
         <v>270</v>
@@ -4518,7 +4527,7 @@
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
-        <v>198</v>
+        <v>142</v>
       </c>
       <c r="B273" s="1" t="s">
         <v>270</v>
@@ -4529,7 +4538,7 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
-        <v>76</v>
+        <v>198</v>
       </c>
       <c r="B274" s="1" t="s">
         <v>270</v>
@@ -4540,7 +4549,7 @@
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B275" s="1" t="s">
         <v>270</v>
@@ -4551,7 +4560,7 @@
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
-        <v>280</v>
+        <v>77</v>
       </c>
       <c r="B276" s="1" t="s">
         <v>270</v>
@@ -4562,7 +4571,7 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>44</v>
+        <v>280</v>
       </c>
       <c r="B277" s="1" t="s">
         <v>270</v>
@@ -4573,7 +4582,7 @@
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
-        <v>318</v>
+        <v>44</v>
       </c>
       <c r="B278" s="1" t="s">
         <v>270</v>
@@ -4584,29 +4593,29 @@
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
-        <v>86</v>
+        <v>318</v>
       </c>
       <c r="B279" s="1" t="s">
         <v>270</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="B280" s="1" t="s">
         <v>270</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B281" s="1" t="s">
         <v>270</v>
@@ -4617,7 +4626,7 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="B282" s="1" t="s">
         <v>270</v>
@@ -4628,7 +4637,7 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
-        <v>294</v>
+        <v>21</v>
       </c>
       <c r="B283" s="1" t="s">
         <v>270</v>
@@ -4639,7 +4648,7 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
-        <v>344</v>
+        <v>294</v>
       </c>
       <c r="B284" s="1" t="s">
         <v>270</v>
@@ -4650,7 +4659,7 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
-        <v>23</v>
+        <v>344</v>
       </c>
       <c r="B285" s="1" t="s">
         <v>270</v>
@@ -4661,7 +4670,7 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>241</v>
+        <v>23</v>
       </c>
       <c r="B286" s="1" t="s">
         <v>270</v>
@@ -4672,7 +4681,7 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
-        <v>214</v>
+        <v>241</v>
       </c>
       <c r="B287" s="1" t="s">
         <v>270</v>
@@ -4683,7 +4692,7 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="B288" s="1" t="s">
         <v>270</v>
@@ -4694,29 +4703,29 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
-        <v>119</v>
+        <v>199</v>
       </c>
       <c r="B289" s="1" t="s">
         <v>270</v>
       </c>
       <c r="C289" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
-        <v>218</v>
+        <v>119</v>
       </c>
       <c r="B290" s="1" t="s">
         <v>270</v>
       </c>
       <c r="C290" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
-        <v>20</v>
+        <v>218</v>
       </c>
       <c r="B291" s="1" t="s">
         <v>270</v>
@@ -4727,32 +4736,32 @@
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="B292" s="1" t="s">
         <v>270</v>
       </c>
       <c r="C292" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="D292" s="1" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
-        <v>210</v>
+        <v>47</v>
       </c>
       <c r="B293" s="1" t="s">
         <v>270</v>
       </c>
       <c r="C293" s="1" t="s">
         <v>272</v>
+      </c>
+      <c r="D293" s="1" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
-        <v>330</v>
+        <v>210</v>
       </c>
       <c r="B294" s="1" t="s">
         <v>270</v>
@@ -4763,7 +4772,7 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
-        <v>353</v>
+        <v>330</v>
       </c>
       <c r="B295" s="1" t="s">
         <v>270</v>
@@ -4774,7 +4783,7 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
-        <v>140</v>
+        <v>353</v>
       </c>
       <c r="B296" s="1" t="s">
         <v>270</v>
@@ -4785,7 +4794,7 @@
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
-        <v>27</v>
+        <v>140</v>
       </c>
       <c r="B297" s="1" t="s">
         <v>270</v>
@@ -4796,7 +4805,7 @@
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
-        <v>184</v>
+        <v>27</v>
       </c>
       <c r="B298" s="1" t="s">
         <v>270</v>
@@ -4807,7 +4816,7 @@
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
-        <v>355</v>
+        <v>184</v>
       </c>
       <c r="B299" s="1" t="s">
         <v>270</v>
@@ -4818,7 +4827,7 @@
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
-        <v>136</v>
+        <v>355</v>
       </c>
       <c r="B300" s="1" t="s">
         <v>270</v>
@@ -4829,29 +4838,29 @@
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
-        <v>237</v>
+        <v>136</v>
       </c>
       <c r="B301" s="1" t="s">
         <v>270</v>
       </c>
       <c r="C301" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="B302" s="1" t="s">
         <v>270</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
-        <v>262</v>
+        <v>230</v>
       </c>
       <c r="B303" s="1" t="s">
         <v>270</v>
@@ -4862,7 +4871,7 @@
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
-        <v>369</v>
+        <v>262</v>
       </c>
       <c r="B304" s="1" t="s">
         <v>270</v>
@@ -4873,7 +4882,7 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
-        <v>35</v>
+        <v>369</v>
       </c>
       <c r="B305" s="1" t="s">
         <v>270</v>
@@ -4884,7 +4893,7 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
-        <v>305</v>
+        <v>35</v>
       </c>
       <c r="B306" s="1" t="s">
         <v>270</v>
@@ -4895,7 +4904,7 @@
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
-        <v>277</v>
+        <v>305</v>
       </c>
       <c r="B307" s="1" t="s">
         <v>270</v>
@@ -4906,32 +4915,32 @@
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
-        <v>7</v>
+        <v>277</v>
       </c>
       <c r="B308" s="1" t="s">
         <v>270</v>
       </c>
       <c r="C308" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="D308" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
-        <v>240</v>
+        <v>7</v>
       </c>
       <c r="B309" s="1" t="s">
         <v>270</v>
       </c>
       <c r="C309" s="1" t="s">
         <v>272</v>
+      </c>
+      <c r="D309" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
-        <v>311</v>
+        <v>240</v>
       </c>
       <c r="B310" s="1" t="s">
         <v>270</v>
@@ -4942,7 +4951,7 @@
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
-        <v>254</v>
+        <v>311</v>
       </c>
       <c r="B311" s="1" t="s">
         <v>270</v>
@@ -4953,7 +4962,7 @@
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B312" s="1" t="s">
         <v>270</v>
@@ -4964,7 +4973,7 @@
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
-        <v>149</v>
+        <v>258</v>
       </c>
       <c r="B313" s="1" t="s">
         <v>270</v>
@@ -4975,7 +4984,7 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
-        <v>265</v>
+        <v>149</v>
       </c>
       <c r="B314" s="1" t="s">
         <v>270</v>
@@ -4986,7 +4995,7 @@
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
-        <v>204</v>
+        <v>265</v>
       </c>
       <c r="B315" s="1" t="s">
         <v>270</v>
@@ -4997,7 +5006,7 @@
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
-        <v>141</v>
+        <v>204</v>
       </c>
       <c r="B316" s="1" t="s">
         <v>270</v>
@@ -5008,7 +5017,7 @@
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
-        <v>48</v>
+        <v>141</v>
       </c>
       <c r="B317" s="1" t="s">
         <v>270</v>
@@ -5019,7 +5028,7 @@
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
-        <v>147</v>
+        <v>48</v>
       </c>
       <c r="B318" s="1" t="s">
         <v>270</v>
@@ -5030,7 +5039,7 @@
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
-        <v>279</v>
+        <v>147</v>
       </c>
       <c r="B319" s="1" t="s">
         <v>270</v>
@@ -5041,362 +5050,362 @@
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C320" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A321" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="B320" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C320" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A321" s="1" t="s">
+      <c r="B321" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C321" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A322" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B321" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C321" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A322" s="1" t="s">
+      <c r="B322" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C322" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A323" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B322" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C322" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A323" s="1" t="s">
+      <c r="B323" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C323" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A324" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="B323" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C323" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A324" s="1" t="s">
+      <c r="B324" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C324" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A325" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B324" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C324" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A325" s="1" t="s">
+      <c r="B325" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C325" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A326" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B325" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C325" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A326" s="1" t="s">
+      <c r="B326" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C326" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A327" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="B326" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C326" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A327" s="1" t="s">
+      <c r="B327" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C327" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A328" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="B327" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C327" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A328" s="1" t="s">
+      <c r="B328" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C328" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A329" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B328" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C328" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A329" s="1" t="s">
+      <c r="B329" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C329" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A330" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="B329" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C329" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A330" s="1" t="s">
+      <c r="B330" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C330" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A331" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B330" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C330" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A331" s="1" t="s">
+      <c r="B331" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C331" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A332" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B331" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C331" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A332" s="1" t="s">
+      <c r="B332" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C332" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A333" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B332" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C332" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A333" s="1" t="s">
+      <c r="B333" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C333" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A334" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B333" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C333" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A334" s="1" t="s">
+      <c r="B334" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C334" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A335" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B334" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C334" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A335" s="1" t="s">
+      <c r="B335" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C335" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A336" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="B335" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C335" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A336" s="1" t="s">
+      <c r="B336" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C336" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A337" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B336" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C336" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="D336" s="1" t="s">
+      <c r="B337" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C337" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D337" s="1" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A337" s="1" t="s">
+    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A338" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B337" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C337" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A338" s="1" t="s">
+      <c r="B338" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A339" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="B338" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C338" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A339" s="1" t="s">
+      <c r="B339" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C339" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A340" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B339" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C339" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A340" s="1" t="s">
+      <c r="B340" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C340" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A341" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B340" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C340" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A341" s="1" t="s">
+      <c r="B341" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C341" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A342" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B341" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C341" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A342" s="1" t="s">
+      <c r="B342" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C342" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A343" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="B342" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C342" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A343" s="1" t="s">
+      <c r="B343" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C343" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A344" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B343" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C343" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A344" s="1" t="s">
+      <c r="B344" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C344" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A345" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B344" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C344" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A345" s="1" t="s">
+      <c r="B345" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C345" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A346" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B345" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C345" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A346" s="1" t="s">
+      <c r="B346" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C346" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A347" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B346" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C346" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A347" s="1" t="s">
+      <c r="B347" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C347" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A348" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="B347" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C347" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A348" s="1" t="s">
+      <c r="B348" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C348" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A349" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B348" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C348" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A349" s="1" t="s">
+      <c r="B349" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C349" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A350" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="B349" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C349" s="1" t="s">
+      <c r="B350" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C350" s="1" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A350" s="1" t="s">
+    <row r="351" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A351" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B350" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C350" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A351" s="1" t="s">
+      <c r="B351" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C351" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="352" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A352" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="B351" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C351" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A352" s="1" t="s">
-        <v>242</v>
       </c>
       <c r="B352" s="1" t="s">
         <v>270</v>
@@ -5407,7 +5416,7 @@
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
-        <v>130</v>
+        <v>242</v>
       </c>
       <c r="B353" s="1" t="s">
         <v>270</v>
@@ -5418,7 +5427,7 @@
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="B354" s="1" t="s">
         <v>270</v>
@@ -5429,7 +5438,7 @@
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
-        <v>312</v>
+        <v>103</v>
       </c>
       <c r="B355" s="1" t="s">
         <v>270</v>
@@ -5440,7 +5449,7 @@
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
-        <v>247</v>
+        <v>312</v>
       </c>
       <c r="B356" s="1" t="s">
         <v>270</v>
@@ -5451,7 +5460,7 @@
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
-        <v>352</v>
+        <v>247</v>
       </c>
       <c r="B357" s="1" t="s">
         <v>270</v>
@@ -5462,7 +5471,7 @@
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
-        <v>106</v>
+        <v>352</v>
       </c>
       <c r="B358" s="1" t="s">
         <v>270</v>
@@ -5473,7 +5482,7 @@
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
-        <v>250</v>
+        <v>106</v>
       </c>
       <c r="B359" s="1" t="s">
         <v>270</v>
@@ -5484,7 +5493,7 @@
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
-        <v>161</v>
+        <v>250</v>
       </c>
       <c r="B360" s="1" t="s">
         <v>270</v>
@@ -5495,12 +5504,23 @@
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B361" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C361" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A362" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B361" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="C361" s="1" t="s">
+      <c r="B362" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C362" s="1" t="s">
         <v>272</v>
       </c>
     </row>

</xml_diff>